<commit_message>
Several fixes and improvements around deleting and renaming
</commit_message>
<xml_diff>
--- a/sample data/LingMetaX_Sessions.xlsx
+++ b/sample data/LingMetaX_Sessions.xlsx
@@ -158,9 +158,6 @@
     <t>session two</t>
   </si>
   <si>
-    <t>this is fun</t>
-  </si>
-  <si>
     <t>Recorder</t>
   </si>
   <si>
@@ -197,8 +194,89 @@
     <t>Vince White</t>
   </si>
   <si>
-    <r>
-      <t>Minim</t>
+    <t>something</t>
+  </si>
+  <si>
+    <t>Conversation</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Zoom</t>
+  </si>
+  <si>
+    <t>สระ</t>
+  </si>
+  <si>
+    <t>Gondwana</t>
+  </si>
+  <si>
+    <t>Rap</t>
+  </si>
+  <si>
+    <t>RC</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>bogus</t>
+  </si>
+  <si>
+    <t>Time Limit</t>
+  </si>
+  <si>
+    <t>Level 1: Public access</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Protected</t>
+  </si>
+  <si>
+    <t>Institution</t>
+  </si>
+  <si>
+    <t>REAP users</t>
+  </si>
+  <si>
+    <t>EnTiTy</t>
+  </si>
+  <si>
+    <t>some reason</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>another explanation</t>
+  </si>
+  <si>
+    <t>Yesterday</t>
+  </si>
+  <si>
+    <t>This one has a bad date</t>
+  </si>
+  <si>
+    <t>foobar</t>
+  </si>
+  <si>
+    <r>
+      <t>Minim qui dolore</t>
     </r>
     <r>
       <rPr>
@@ -216,7 +294,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>qui</t>
+      <t>ex</t>
     </r>
     <r>
       <rPr>
@@ -234,6 +312,114 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
+      <t>eu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>pariatur</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>eu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>cupidatat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>sint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>esse</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
       <t>dolore</t>
     </r>
     <r>
@@ -252,7 +438,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>ex</t>
+      <t>elit</t>
     </r>
     <r>
       <rPr>
@@ -270,7 +456,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>eu</t>
+      <t>labore</t>
     </r>
     <r>
       <rPr>
@@ -288,7 +474,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>pariatur</t>
+      <t>proident</t>
     </r>
     <r>
       <rPr>
@@ -306,7 +492,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>eu</t>
+      <t>officia</t>
     </r>
     <r>
       <rPr>
@@ -315,240 +501,18 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>cupidatat</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>sint</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>esse</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>dolore</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>elit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>labore</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>proident</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>officia</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
       <t>.</t>
     </r>
   </si>
   <si>
-    <t>something</t>
-  </si>
-  <si>
-    <t>Conversation</t>
-  </si>
-  <si>
-    <t>Australia</t>
-  </si>
-  <si>
-    <t>Zoom</t>
-  </si>
-  <si>
-    <t>สระ</t>
-  </si>
-  <si>
-    <t>Gondwana</t>
-  </si>
-  <si>
-    <t>Rap</t>
-  </si>
-  <si>
-    <t>RC</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>bogus</t>
-  </si>
-  <si>
-    <t>Time Limit</t>
-  </si>
-  <si>
-    <t>Level 1: Public access</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Protected</t>
-  </si>
-  <si>
-    <t>Institution</t>
-  </si>
-  <si>
-    <t>REAP users</t>
-  </si>
-  <si>
-    <t>EnTiTy</t>
-  </si>
-  <si>
-    <t>some reason</t>
-  </si>
-  <si>
-    <t>red</t>
-  </si>
-  <si>
-    <t>green</t>
-  </si>
-  <si>
-    <t>another explanation</t>
-  </si>
-  <si>
-    <t>Yesterday</t>
-  </si>
-  <si>
-    <t>This one has a bad date</t>
-  </si>
-  <si>
-    <t>foobar</t>
+    <t>hɛˈləʊ wɜːld</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -593,6 +557,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF373737"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -614,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -626,6 +596,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -909,9 +880,9 @@
   <dimension ref="A1:AQ7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="18555" topLeftCell="M1"/>
-      <selection activeCell="C11" sqref="C11"/>
-      <selection pane="topRight" activeCell="M38" sqref="M38"/>
+      <pane xSplit="18555" topLeftCell="M1" activePane="topRight"/>
+      <selection activeCell="B6" sqref="A1:S7"/>
+      <selection pane="topRight" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,103 +1043,103 @@
         <v>44357</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
         <v>42</v>
       </c>
       <c r="D2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>68</v>
       </c>
-      <c r="G2" t="s">
-        <v>70</v>
-      </c>
       <c r="H2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="K2" t="s">
         <v>77</v>
       </c>
-      <c r="K2" t="s">
-        <v>79</v>
-      </c>
       <c r="L2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD2" t="s">
         <v>59</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>61</v>
-      </c>
       <c r="AH2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ2" t="s">
         <v>51</v>
       </c>
-      <c r="AI2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AJ2" t="s">
+      <c r="AL2" t="s">
         <v>52</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AN2" t="s">
         <v>53</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AP2" t="s">
         <v>54</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
         <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M3" t="s">
-        <v>64</v>
-      </c>
-      <c r="N3" t="s">
-        <v>44</v>
+        <v>62</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>84</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AH3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.25">
@@ -1176,22 +1147,22 @@
         <v>44084</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="AH4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AI4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.25">
@@ -1199,13 +1170,13 @@
         <v>44085</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AI5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.25">
@@ -1213,21 +1184,21 @@
         <v>44086</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" t="s">
         <v>82</v>
-      </c>
-      <c r="B7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Get excel dates in an unambiguous way
Note, I didn't do anything with CSV dates
</commit_message>
<xml_diff>
--- a/sample data/LingMetaX_Sessions.xlsx
+++ b/sample data/LingMetaX_Sessions.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\lameta\sample data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448AA796-D2FB-490B-9AB8-9EB6B126C973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28065" windowHeight="12165"/>
+    <workbookView xWindow="-25155" yWindow="765" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -511,7 +512,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -876,12 +877,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="18555" topLeftCell="M1" activePane="topRight"/>
-      <selection activeCell="B6" sqref="A1:S7"/>
+      <pane xSplit="18555" topLeftCell="M1"/>
+      <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
@@ -1040,7 +1041,7 @@
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>44357</v>
+        <v>44367</v>
       </c>
       <c r="B2" t="s">
         <v>46</v>

</xml_diff>